<commit_message>
update ac3 and skills
</commit_message>
<xml_diff>
--- a/Personal/skill.xlsx
+++ b/Personal/skill.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
   <si>
     <t>grub</t>
   </si>
@@ -157,6 +157,66 @@
   </si>
   <si>
     <t>php</t>
+  </si>
+  <si>
+    <t>virtual machine</t>
+  </si>
+  <si>
+    <t>docker</t>
+  </si>
+  <si>
+    <t>zookeeper</t>
+  </si>
+  <si>
+    <t>go</t>
+  </si>
+  <si>
+    <t>ajax</t>
+  </si>
+  <si>
+    <t>django</t>
+  </si>
+  <si>
+    <t>perl</t>
+  </si>
+  <si>
+    <t>algorithm</t>
+  </si>
+  <si>
+    <t>testimony / certification</t>
+  </si>
+  <si>
+    <t>projects</t>
+  </si>
+  <si>
+    <t>gsm</t>
+  </si>
+  <si>
+    <t>lte</t>
+  </si>
+  <si>
+    <t>Windows GUI</t>
+  </si>
+  <si>
+    <t>Linux GUI</t>
+  </si>
+  <si>
+    <t>purify</t>
+  </si>
+  <si>
+    <t>PureCoverage</t>
+  </si>
+  <si>
+    <t>wireshark</t>
+  </si>
+  <si>
+    <t>netfilter/iptables</t>
+  </si>
+  <si>
+    <t>MAC OSX</t>
+  </si>
+  <si>
+    <t>iOS dev</t>
   </si>
 </sst>
 </file>
@@ -495,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,9 +567,10 @@
     <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -522,8 +583,14 @@
       <c r="D1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -531,7 +598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -539,7 +606,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -547,7 +614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -555,7 +622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -563,7 +630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -571,7 +638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -579,42 +646,42 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -749,8 +816,102 @@
         <v>46</v>
       </c>
     </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A56" r:id="rId1" display="http://www.ltesting.net/ceshi/ceshijishu/rjcsgj/rational/purecoverage/"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>